<commit_message>
multiplicadors a medi modificats
</commit_message>
<xml_diff>
--- a/inputs compound generator/inputs/atenuacions_generacions.xlsx
+++ b/inputs compound generator/inputs/atenuacions_generacions.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jsalo\PycharmProjects\traca\inputs compound generator\inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44C19101-7F44-4438-B56E-BC6FD07314D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D93434D9-8503-435D-B8C3-F4EE2391860A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="12220" xr2:uid="{3E496A17-2DFC-444D-AF2A-2E041A081BD5}"/>
   </bookViews>
@@ -64,12 +64,6 @@
     <t>CNP</t>
   </si>
   <si>
-    <t>Arsènic dissolt</t>
-  </si>
-  <si>
-    <t>Crom dissolt</t>
-  </si>
-  <si>
     <t>1.1.1-Tricloroetà</t>
   </si>
   <si>
@@ -94,9 +88,6 @@
     <t>Benzo(b)fluorantè</t>
   </si>
   <si>
-    <t>Cadmi dissolt</t>
-  </si>
-  <si>
     <t>Tetraclorur de carboni</t>
   </si>
   <si>
@@ -115,9 +106,6 @@
     <t>Clotrimazol</t>
   </si>
   <si>
-    <t>Coure dissolt</t>
-  </si>
-  <si>
     <t>Diclorobenzè</t>
   </si>
   <si>
@@ -169,12 +157,6 @@
     <t>Isoproturon</t>
   </si>
   <si>
-    <t>Plom dissolt</t>
-  </si>
-  <si>
-    <t>Mercuri dissolt</t>
-  </si>
-  <si>
     <t>Metolaclor</t>
   </si>
   <si>
@@ -184,9 +166,6 @@
     <t>Naftalè</t>
   </si>
   <si>
-    <t>Niquel dissolt</t>
-  </si>
-  <si>
     <t>Nonilfenols</t>
   </si>
   <si>
@@ -241,9 +220,6 @@
     <t>Xilè</t>
   </si>
   <si>
-    <t>Zinc dissolt</t>
-  </si>
-  <si>
     <t>contaminant</t>
   </si>
   <si>
@@ -293,6 +269,30 @@
   </si>
   <si>
     <t>AOP</t>
+  </si>
+  <si>
+    <t>Arsènic</t>
+  </si>
+  <si>
+    <t>Cadmi</t>
+  </si>
+  <si>
+    <t>Crom</t>
+  </si>
+  <si>
+    <t>Plom</t>
+  </si>
+  <si>
+    <t>Niquel</t>
+  </si>
+  <si>
+    <t>Zinc</t>
+  </si>
+  <si>
+    <t>Coure</t>
+  </si>
+  <si>
+    <t>Mercuri</t>
   </si>
 </sst>
 </file>
@@ -345,40 +345,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -695,8 +668,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0BE9104B-031B-40A3-A03F-BC2098EC6758}">
   <dimension ref="A1:P71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="G29" sqref="G29"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A24" sqref="A24:XFD24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -707,7 +680,7 @@
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -722,16 +695,16 @@
         <v>3</v>
       </c>
       <c r="F1" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="G1" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="H1" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="I1" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="J1" t="s">
         <v>4</v>
@@ -749,15 +722,15 @@
         <v>8</v>
       </c>
       <c r="O1" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="P1" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B2">
         <v>0</v>
@@ -771,16 +744,16 @@
       <c r="E2" s="1">
         <v>10</v>
       </c>
-      <c r="F2" s="32">
-        <v>0</v>
-      </c>
-      <c r="G2" s="32">
-        <v>0</v>
-      </c>
-      <c r="H2" s="32">
-        <v>0</v>
-      </c>
-      <c r="I2" s="32">
+      <c r="F2" s="1">
+        <v>0</v>
+      </c>
+      <c r="G2" s="1">
+        <v>0</v>
+      </c>
+      <c r="H2" s="1">
+        <v>0</v>
+      </c>
+      <c r="I2" s="1">
         <v>0</v>
       </c>
       <c r="J2">
@@ -807,7 +780,7 @@
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B3">
         <v>0</v>
@@ -821,16 +794,16 @@
       <c r="E3">
         <v>0</v>
       </c>
-      <c r="F3" s="32">
-        <v>0</v>
-      </c>
-      <c r="G3" s="32">
-        <v>0</v>
-      </c>
-      <c r="H3" s="32">
-        <v>0</v>
-      </c>
-      <c r="I3" s="32">
+      <c r="F3" s="1">
+        <v>0</v>
+      </c>
+      <c r="G3" s="1">
+        <v>0</v>
+      </c>
+      <c r="H3" s="1">
+        <v>0</v>
+      </c>
+      <c r="I3" s="1">
         <v>0</v>
       </c>
       <c r="J3">
@@ -857,7 +830,7 @@
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B4">
         <v>0</v>
@@ -871,16 +844,16 @@
       <c r="E4">
         <v>0</v>
       </c>
-      <c r="F4" s="32">
-        <v>0</v>
-      </c>
-      <c r="G4" s="32">
-        <v>0</v>
-      </c>
-      <c r="H4" s="32">
-        <v>0</v>
-      </c>
-      <c r="I4" s="32">
+      <c r="F4" s="1">
+        <v>0</v>
+      </c>
+      <c r="G4" s="1">
+        <v>0</v>
+      </c>
+      <c r="H4" s="1">
+        <v>0</v>
+      </c>
+      <c r="I4" s="1">
         <v>0</v>
       </c>
       <c r="J4">
@@ -907,7 +880,7 @@
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B5">
         <v>5.376283863420694</v>
@@ -921,16 +894,16 @@
       <c r="E5">
         <v>0</v>
       </c>
-      <c r="F5" s="32">
-        <v>0</v>
-      </c>
-      <c r="G5" s="32">
-        <v>0</v>
-      </c>
-      <c r="H5" s="32">
-        <v>0</v>
-      </c>
-      <c r="I5" s="32">
+      <c r="F5" s="1">
+        <v>0</v>
+      </c>
+      <c r="G5" s="1">
+        <v>0</v>
+      </c>
+      <c r="H5" s="1">
+        <v>0</v>
+      </c>
+      <c r="I5" s="1">
         <v>0</v>
       </c>
       <c r="J5">
@@ -957,7 +930,7 @@
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B6">
         <v>0</v>
@@ -971,16 +944,16 @@
       <c r="E6">
         <v>0</v>
       </c>
-      <c r="F6" s="32">
-        <v>0</v>
-      </c>
-      <c r="G6" s="32">
-        <v>0</v>
-      </c>
-      <c r="H6" s="32">
-        <v>0</v>
-      </c>
-      <c r="I6" s="32">
+      <c r="F6" s="1">
+        <v>0</v>
+      </c>
+      <c r="G6" s="1">
+        <v>0</v>
+      </c>
+      <c r="H6" s="1">
+        <v>0</v>
+      </c>
+      <c r="I6" s="1">
         <v>0</v>
       </c>
       <c r="J6">
@@ -1007,7 +980,7 @@
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B7">
         <v>7.948300628203997</v>
@@ -1021,16 +994,16 @@
       <c r="E7">
         <v>0</v>
       </c>
-      <c r="F7" s="32">
-        <v>0</v>
-      </c>
-      <c r="G7" s="32">
-        <v>0</v>
-      </c>
-      <c r="H7" s="32">
-        <v>0</v>
-      </c>
-      <c r="I7" s="32">
+      <c r="F7" s="1">
+        <v>0</v>
+      </c>
+      <c r="G7" s="1">
+        <v>0</v>
+      </c>
+      <c r="H7" s="1">
+        <v>0</v>
+      </c>
+      <c r="I7" s="1">
         <v>0</v>
       </c>
       <c r="J7">
@@ -1057,7 +1030,7 @@
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>9</v>
+        <v>78</v>
       </c>
       <c r="B8">
         <v>0</v>
@@ -1071,16 +1044,16 @@
       <c r="E8">
         <v>0</v>
       </c>
-      <c r="F8" s="32">
-        <v>0</v>
-      </c>
-      <c r="G8" s="32">
-        <v>0</v>
-      </c>
-      <c r="H8" s="32">
-        <v>0</v>
-      </c>
-      <c r="I8" s="32">
+      <c r="F8" s="1">
+        <v>0</v>
+      </c>
+      <c r="G8" s="1">
+        <v>0</v>
+      </c>
+      <c r="H8" s="1">
+        <v>0</v>
+      </c>
+      <c r="I8" s="1">
         <v>0</v>
       </c>
       <c r="J8">
@@ -1111,7 +1084,7 @@
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B9">
         <v>7.5301826061777488</v>
@@ -1125,16 +1098,16 @@
       <c r="E9">
         <v>10</v>
       </c>
-      <c r="F9" s="32">
-        <v>0</v>
-      </c>
-      <c r="G9" s="32">
-        <v>0</v>
-      </c>
-      <c r="H9" s="32">
-        <v>0</v>
-      </c>
-      <c r="I9" s="32">
+      <c r="F9" s="1">
+        <v>0</v>
+      </c>
+      <c r="G9" s="1">
+        <v>0</v>
+      </c>
+      <c r="H9" s="1">
+        <v>0</v>
+      </c>
+      <c r="I9" s="1">
         <v>0</v>
       </c>
       <c r="J9">
@@ -1161,7 +1134,7 @@
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B10">
         <v>0</v>
@@ -1175,16 +1148,16 @@
       <c r="E10" s="1">
         <v>10</v>
       </c>
-      <c r="F10" s="32">
-        <v>0</v>
-      </c>
-      <c r="G10" s="32">
-        <v>0</v>
-      </c>
-      <c r="H10" s="32">
-        <v>0</v>
-      </c>
-      <c r="I10" s="32">
+      <c r="F10" s="1">
+        <v>0</v>
+      </c>
+      <c r="G10" s="1">
+        <v>0</v>
+      </c>
+      <c r="H10" s="1">
+        <v>0</v>
+      </c>
+      <c r="I10" s="1">
         <v>0</v>
       </c>
       <c r="J10">
@@ -1211,7 +1184,7 @@
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>19</v>
+        <v>79</v>
       </c>
       <c r="B11" s="1">
         <v>10</v>
@@ -1225,16 +1198,16 @@
       <c r="E11" s="1">
         <v>10</v>
       </c>
-      <c r="F11" s="32">
-        <v>0</v>
-      </c>
-      <c r="G11" s="32">
-        <v>0</v>
-      </c>
-      <c r="H11" s="32">
-        <v>0</v>
-      </c>
-      <c r="I11" s="32">
+      <c r="F11" s="1">
+        <v>0</v>
+      </c>
+      <c r="G11" s="1">
+        <v>0</v>
+      </c>
+      <c r="H11" s="1">
+        <v>0</v>
+      </c>
+      <c r="I11" s="1">
         <v>0</v>
       </c>
       <c r="J11" s="1">
@@ -1261,7 +1234,7 @@
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B12">
         <v>0</v>
@@ -1275,16 +1248,16 @@
       <c r="E12">
         <v>0</v>
       </c>
-      <c r="F12" s="32">
-        <v>0</v>
-      </c>
-      <c r="G12" s="32">
-        <v>0</v>
-      </c>
-      <c r="H12" s="32">
-        <v>0</v>
-      </c>
-      <c r="I12" s="32">
+      <c r="F12" s="1">
+        <v>0</v>
+      </c>
+      <c r="G12" s="1">
+        <v>0</v>
+      </c>
+      <c r="H12" s="1">
+        <v>0</v>
+      </c>
+      <c r="I12" s="1">
         <v>0</v>
       </c>
       <c r="J12">
@@ -1311,7 +1284,7 @@
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B13">
         <v>0</v>
@@ -1325,16 +1298,16 @@
       <c r="E13">
         <v>0</v>
       </c>
-      <c r="F13" s="6">
+      <c r="F13" s="1">
         <v>70</v>
       </c>
-      <c r="G13" s="6">
+      <c r="G13" s="1">
         <v>90</v>
       </c>
-      <c r="H13" s="6">
+      <c r="H13" s="1">
         <v>80</v>
       </c>
-      <c r="I13" s="6">
+      <c r="I13" s="1">
         <v>90</v>
       </c>
       <c r="J13">
@@ -1361,7 +1334,7 @@
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B14">
         <v>0.54161556151880452</v>
@@ -1375,16 +1348,16 @@
       <c r="E14">
         <v>0</v>
       </c>
-      <c r="F14" s="32">
-        <v>0</v>
-      </c>
-      <c r="G14" s="32">
-        <v>0</v>
-      </c>
-      <c r="H14" s="32">
-        <v>0</v>
-      </c>
-      <c r="I14" s="32">
+      <c r="F14" s="1">
+        <v>0</v>
+      </c>
+      <c r="G14" s="1">
+        <v>0</v>
+      </c>
+      <c r="H14" s="1">
+        <v>0</v>
+      </c>
+      <c r="I14" s="1">
         <v>0</v>
       </c>
       <c r="J14">
@@ -1411,7 +1384,7 @@
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>10</v>
+        <v>80</v>
       </c>
       <c r="B15">
         <v>10</v>
@@ -1425,16 +1398,16 @@
       <c r="E15">
         <v>10</v>
       </c>
-      <c r="F15" s="32">
-        <v>0</v>
-      </c>
-      <c r="G15" s="32">
-        <v>0</v>
-      </c>
-      <c r="H15" s="32">
-        <v>0</v>
-      </c>
-      <c r="I15" s="32">
+      <c r="F15" s="1">
+        <v>0</v>
+      </c>
+      <c r="G15" s="1">
+        <v>0</v>
+      </c>
+      <c r="H15" s="1">
+        <v>0</v>
+      </c>
+      <c r="I15" s="1">
         <v>0</v>
       </c>
       <c r="J15">
@@ -1465,7 +1438,7 @@
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B16">
         <v>10.06138234998703</v>
@@ -1479,16 +1452,16 @@
       <c r="E16">
         <v>0</v>
       </c>
-      <c r="F16" s="7">
+      <c r="F16" s="1">
         <v>90</v>
       </c>
-      <c r="G16" s="7">
+      <c r="G16" s="1">
         <v>98</v>
       </c>
-      <c r="H16" s="7">
+      <c r="H16" s="1">
         <v>90</v>
       </c>
-      <c r="I16" s="7">
+      <c r="I16" s="1">
         <v>90</v>
       </c>
       <c r="J16" s="1">
@@ -1515,7 +1488,7 @@
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B17">
         <v>0</v>
@@ -1529,16 +1502,16 @@
       <c r="E17">
         <v>0</v>
       </c>
-      <c r="F17" s="32">
+      <c r="F17" s="1">
         <v>58.62</v>
       </c>
-      <c r="G17" s="32">
+      <c r="G17" s="1">
         <v>92.13</v>
       </c>
-      <c r="H17" s="32">
+      <c r="H17" s="1">
         <v>50</v>
       </c>
-      <c r="I17" s="32">
+      <c r="I17" s="1">
         <v>52.88</v>
       </c>
       <c r="J17">
@@ -1565,7 +1538,7 @@
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B18">
         <v>0</v>
@@ -1579,16 +1552,16 @@
       <c r="E18">
         <v>0</v>
       </c>
-      <c r="F18" s="32">
-        <v>0</v>
-      </c>
-      <c r="G18" s="32">
-        <v>0</v>
-      </c>
-      <c r="H18" s="32">
-        <v>0</v>
-      </c>
-      <c r="I18" s="32">
+      <c r="F18" s="1">
+        <v>0</v>
+      </c>
+      <c r="G18" s="1">
+        <v>0</v>
+      </c>
+      <c r="H18" s="1">
+        <v>0</v>
+      </c>
+      <c r="I18" s="1">
         <v>0</v>
       </c>
       <c r="J18">
@@ -1615,7 +1588,7 @@
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>26</v>
+        <v>84</v>
       </c>
       <c r="B19">
         <v>10</v>
@@ -1629,16 +1602,16 @@
       <c r="E19">
         <v>0</v>
       </c>
-      <c r="F19" s="8">
+      <c r="F19" s="1">
         <v>30</v>
       </c>
-      <c r="G19" s="8">
+      <c r="G19" s="1">
         <v>98</v>
       </c>
-      <c r="H19" s="8">
-        <v>0</v>
-      </c>
-      <c r="I19" s="8">
+      <c r="H19" s="1">
+        <v>0</v>
+      </c>
+      <c r="I19" s="1">
         <v>0</v>
       </c>
       <c r="J19">
@@ -1669,7 +1642,7 @@
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="B20">
         <v>3.4635692704713561</v>
@@ -1683,16 +1656,16 @@
       <c r="E20">
         <v>0</v>
       </c>
-      <c r="F20" s="32">
-        <v>0</v>
-      </c>
-      <c r="G20" s="32">
-        <v>0</v>
-      </c>
-      <c r="H20" s="32">
-        <v>0</v>
-      </c>
-      <c r="I20" s="32">
+      <c r="F20" s="1">
+        <v>0</v>
+      </c>
+      <c r="G20" s="1">
+        <v>0</v>
+      </c>
+      <c r="H20" s="1">
+        <v>0</v>
+      </c>
+      <c r="I20" s="1">
         <v>0</v>
       </c>
       <c r="J20">
@@ -1719,7 +1692,7 @@
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B21">
         <v>0</v>
@@ -1733,16 +1706,16 @@
       <c r="E21">
         <v>0</v>
       </c>
-      <c r="F21" s="32">
-        <v>0</v>
-      </c>
-      <c r="G21" s="32">
-        <v>0</v>
-      </c>
-      <c r="H21" s="32">
-        <v>0</v>
-      </c>
-      <c r="I21" s="32">
+      <c r="F21" s="1">
+        <v>0</v>
+      </c>
+      <c r="G21" s="1">
+        <v>0</v>
+      </c>
+      <c r="H21" s="1">
+        <v>0</v>
+      </c>
+      <c r="I21" s="1">
         <v>0</v>
       </c>
       <c r="J21">
@@ -1769,7 +1742,7 @@
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B22">
         <v>0</v>
@@ -1783,16 +1756,16 @@
       <c r="E22">
         <v>0</v>
       </c>
-      <c r="F22" s="32">
-        <v>0</v>
-      </c>
-      <c r="G22" s="32">
-        <v>0</v>
-      </c>
-      <c r="H22" s="32">
-        <v>0</v>
-      </c>
-      <c r="I22" s="32">
+      <c r="F22" s="1">
+        <v>0</v>
+      </c>
+      <c r="G22" s="1">
+        <v>0</v>
+      </c>
+      <c r="H22" s="1">
+        <v>0</v>
+      </c>
+      <c r="I22" s="1">
         <v>0</v>
       </c>
       <c r="J22">
@@ -1819,7 +1792,7 @@
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="B23">
         <v>0</v>
@@ -1833,16 +1806,16 @@
       <c r="E23">
         <v>0</v>
       </c>
-      <c r="F23" s="32">
-        <v>0</v>
-      </c>
-      <c r="G23" s="32">
-        <v>0</v>
-      </c>
-      <c r="H23" s="32">
-        <v>0</v>
-      </c>
-      <c r="I23" s="32">
+      <c r="F23" s="1">
+        <v>0</v>
+      </c>
+      <c r="G23" s="1">
+        <v>0</v>
+      </c>
+      <c r="H23" s="1">
+        <v>0</v>
+      </c>
+      <c r="I23" s="1">
         <v>0</v>
       </c>
       <c r="J23">
@@ -1869,33 +1842,30 @@
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="B24">
-        <f>100-100*0.971113</f>
-        <v>2.8887</v>
+        <v>4.1900000000000004</v>
       </c>
       <c r="C24">
-        <f>100-100*0.982831</f>
-        <v>1.7168999999999954</v>
+        <v>0</v>
       </c>
       <c r="D24">
         <v>0</v>
       </c>
       <c r="E24">
-        <f>100-100*0.952608</f>
-        <v>4.7391999999999967</v>
-      </c>
-      <c r="F24" s="32">
+        <v>9.9</v>
+      </c>
+      <c r="F24" s="1">
         <v>58.62</v>
       </c>
-      <c r="G24" s="32">
+      <c r="G24" s="1">
         <v>92.13</v>
       </c>
-      <c r="H24" s="32">
+      <c r="H24" s="1">
         <v>50</v>
       </c>
-      <c r="I24" s="32">
+      <c r="I24" s="1">
         <v>52.88</v>
       </c>
       <c r="J24">
@@ -1914,15 +1884,15 @@
         <v>0</v>
       </c>
       <c r="O24" s="4">
-        <v>3.2039499999999997E-5</v>
+        <v>5.2167799999999999E-5</v>
       </c>
       <c r="P24">
-        <v>1</v>
+        <v>11.263199999999999</v>
       </c>
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B25">
         <v>0</v>
@@ -1936,16 +1906,16 @@
       <c r="E25">
         <v>0</v>
       </c>
-      <c r="F25" s="32">
-        <v>0</v>
-      </c>
-      <c r="G25" s="32">
-        <v>0</v>
-      </c>
-      <c r="H25" s="32">
-        <v>0</v>
-      </c>
-      <c r="I25" s="32">
+      <c r="F25" s="1">
+        <v>0</v>
+      </c>
+      <c r="G25" s="1">
+        <v>0</v>
+      </c>
+      <c r="H25" s="1">
+        <v>0</v>
+      </c>
+      <c r="I25" s="1">
         <v>0</v>
       </c>
       <c r="J25">
@@ -1972,7 +1942,7 @@
     </row>
     <row r="26" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="B26">
         <v>0</v>
@@ -1986,16 +1956,16 @@
       <c r="E26">
         <v>0</v>
       </c>
-      <c r="F26" s="32">
-        <v>0</v>
-      </c>
-      <c r="G26" s="32">
-        <v>0</v>
-      </c>
-      <c r="H26" s="32">
-        <v>0</v>
-      </c>
-      <c r="I26" s="32">
+      <c r="F26" s="1">
+        <v>0</v>
+      </c>
+      <c r="G26" s="1">
+        <v>0</v>
+      </c>
+      <c r="H26" s="1">
+        <v>0</v>
+      </c>
+      <c r="I26" s="1">
         <v>0</v>
       </c>
       <c r="J26">
@@ -2022,7 +1992,7 @@
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="B27">
         <v>0</v>
@@ -2036,16 +2006,16 @@
       <c r="E27">
         <v>0</v>
       </c>
-      <c r="F27" s="32">
-        <v>0</v>
-      </c>
-      <c r="G27" s="32">
-        <v>0</v>
-      </c>
-      <c r="H27" s="32">
-        <v>0</v>
-      </c>
-      <c r="I27" s="32">
+      <c r="F27" s="1">
+        <v>0</v>
+      </c>
+      <c r="G27" s="1">
+        <v>0</v>
+      </c>
+      <c r="H27" s="1">
+        <v>0</v>
+      </c>
+      <c r="I27" s="1">
         <v>0</v>
       </c>
       <c r="J27">
@@ -2072,7 +2042,7 @@
     </row>
     <row r="28" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="B28">
         <v>0</v>
@@ -2086,16 +2056,16 @@
       <c r="E28">
         <v>0</v>
       </c>
-      <c r="F28" s="32">
-        <v>0</v>
-      </c>
-      <c r="G28" s="32">
-        <v>0</v>
-      </c>
-      <c r="H28" s="32">
-        <v>0</v>
-      </c>
-      <c r="I28" s="32">
+      <c r="F28" s="1">
+        <v>0</v>
+      </c>
+      <c r="G28" s="1">
+        <v>0</v>
+      </c>
+      <c r="H28" s="1">
+        <v>0</v>
+      </c>
+      <c r="I28" s="1">
         <v>0</v>
       </c>
       <c r="J28">
@@ -2122,7 +2092,7 @@
     </row>
     <row r="29" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="B29">
         <v>7.0022257675136252</v>
@@ -2136,16 +2106,16 @@
       <c r="E29">
         <v>0</v>
       </c>
-      <c r="F29" s="32">
-        <v>0</v>
-      </c>
-      <c r="G29" s="32">
-        <v>0</v>
-      </c>
-      <c r="H29" s="32">
-        <v>0</v>
-      </c>
-      <c r="I29" s="32">
+      <c r="F29" s="1">
+        <v>0</v>
+      </c>
+      <c r="G29" s="1">
+        <v>0</v>
+      </c>
+      <c r="H29" s="1">
+        <v>0</v>
+      </c>
+      <c r="I29" s="1">
         <v>0</v>
       </c>
       <c r="J29" s="1">
@@ -2172,7 +2142,7 @@
     </row>
     <row r="30" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="B30">
         <v>0</v>
@@ -2186,16 +2156,16 @@
       <c r="E30">
         <v>0</v>
       </c>
-      <c r="F30" s="32">
-        <v>0</v>
-      </c>
-      <c r="G30" s="32">
-        <v>0</v>
-      </c>
-      <c r="H30" s="32">
-        <v>0</v>
-      </c>
-      <c r="I30" s="32">
+      <c r="F30" s="1">
+        <v>0</v>
+      </c>
+      <c r="G30" s="1">
+        <v>0</v>
+      </c>
+      <c r="H30" s="1">
+        <v>0</v>
+      </c>
+      <c r="I30" s="1">
         <v>0</v>
       </c>
       <c r="J30">
@@ -2226,7 +2196,7 @@
     </row>
     <row r="31" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="B31">
         <v>0</v>
@@ -2240,16 +2210,16 @@
       <c r="E31">
         <v>0</v>
       </c>
-      <c r="F31" s="32">
-        <v>0</v>
-      </c>
-      <c r="G31" s="32">
-        <v>0</v>
-      </c>
-      <c r="H31" s="32">
-        <v>0</v>
-      </c>
-      <c r="I31" s="32">
+      <c r="F31" s="1">
+        <v>0</v>
+      </c>
+      <c r="G31" s="1">
+        <v>0</v>
+      </c>
+      <c r="H31" s="1">
+        <v>0</v>
+      </c>
+      <c r="I31" s="1">
         <v>0</v>
       </c>
       <c r="J31">
@@ -2276,7 +2246,7 @@
     </row>
     <row r="32" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="B32">
         <v>0</v>
@@ -2290,16 +2260,16 @@
       <c r="E32">
         <v>0</v>
       </c>
-      <c r="F32" s="9">
+      <c r="F32" s="1">
         <v>98</v>
       </c>
-      <c r="G32" s="9">
+      <c r="G32" s="1">
         <v>98</v>
       </c>
-      <c r="H32" s="9">
+      <c r="H32" s="1">
         <v>50</v>
       </c>
-      <c r="I32" s="9">
+      <c r="I32" s="1">
         <v>90</v>
       </c>
       <c r="J32">
@@ -2326,7 +2296,7 @@
     </row>
     <row r="33" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="B33">
         <v>0</v>
@@ -2340,16 +2310,16 @@
       <c r="E33" s="1">
         <v>10</v>
       </c>
-      <c r="F33" s="32">
-        <v>0</v>
-      </c>
-      <c r="G33" s="32">
-        <v>0</v>
-      </c>
-      <c r="H33" s="32">
-        <v>0</v>
-      </c>
-      <c r="I33" s="32">
+      <c r="F33" s="1">
+        <v>0</v>
+      </c>
+      <c r="G33" s="1">
+        <v>0</v>
+      </c>
+      <c r="H33" s="1">
+        <v>0</v>
+      </c>
+      <c r="I33" s="1">
         <v>0</v>
       </c>
       <c r="J33" s="5">
@@ -2376,7 +2346,7 @@
     </row>
     <row r="34" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="B34">
         <v>0</v>
@@ -2390,16 +2360,16 @@
       <c r="E34">
         <v>0</v>
       </c>
-      <c r="F34" s="32">
-        <v>0</v>
-      </c>
-      <c r="G34" s="32">
-        <v>0</v>
-      </c>
-      <c r="H34" s="32">
-        <v>0</v>
-      </c>
-      <c r="I34" s="32">
+      <c r="F34" s="1">
+        <v>0</v>
+      </c>
+      <c r="G34" s="1">
+        <v>0</v>
+      </c>
+      <c r="H34" s="1">
+        <v>0</v>
+      </c>
+      <c r="I34" s="1">
         <v>0</v>
       </c>
       <c r="J34">
@@ -2426,7 +2396,7 @@
     </row>
     <row r="35" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="B35">
         <v>0</v>
@@ -2440,16 +2410,16 @@
       <c r="E35">
         <v>0</v>
       </c>
-      <c r="F35" s="32">
-        <v>0</v>
-      </c>
-      <c r="G35" s="32">
-        <v>0</v>
-      </c>
-      <c r="H35" s="32">
-        <v>0</v>
-      </c>
-      <c r="I35" s="32">
+      <c r="F35" s="1">
+        <v>0</v>
+      </c>
+      <c r="G35" s="1">
+        <v>0</v>
+      </c>
+      <c r="H35" s="1">
+        <v>0</v>
+      </c>
+      <c r="I35" s="1">
         <v>0</v>
       </c>
       <c r="J35">
@@ -2476,7 +2446,7 @@
     </row>
     <row r="36" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="B36">
         <v>0.59688365342226435</v>
@@ -2490,16 +2460,16 @@
       <c r="E36">
         <v>0</v>
       </c>
-      <c r="F36" s="32">
-        <v>0</v>
-      </c>
-      <c r="G36" s="32">
-        <v>0</v>
-      </c>
-      <c r="H36" s="32">
-        <v>0</v>
-      </c>
-      <c r="I36" s="32">
+      <c r="F36" s="1">
+        <v>0</v>
+      </c>
+      <c r="G36" s="1">
+        <v>0</v>
+      </c>
+      <c r="H36" s="1">
+        <v>0</v>
+      </c>
+      <c r="I36" s="1">
         <v>0</v>
       </c>
       <c r="J36">
@@ -2526,7 +2496,7 @@
     </row>
     <row r="37" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
-        <v>44</v>
+        <v>81</v>
       </c>
       <c r="B37">
         <v>0</v>
@@ -2538,49 +2508,45 @@
         <v>0</v>
       </c>
       <c r="E37">
-        <v>0</v>
-      </c>
-      <c r="F37" s="32">
-        <v>58.62</v>
-      </c>
-      <c r="G37" s="32">
-        <v>92.13</v>
-      </c>
-      <c r="H37" s="32">
-        <v>50</v>
-      </c>
-      <c r="I37" s="32">
-        <v>52.88</v>
+        <v>1.7</v>
+      </c>
+      <c r="F37">
+        <v>55</v>
+      </c>
+      <c r="G37" s="1">
+        <v>98</v>
+      </c>
+      <c r="H37" s="1">
+        <v>0</v>
+      </c>
+      <c r="I37" s="1">
+        <v>0</v>
       </c>
       <c r="J37">
         <v>0</v>
       </c>
       <c r="K37">
-        <f>100-51.817</f>
-        <v>48.183</v>
+        <v>55.5</v>
       </c>
       <c r="L37">
-        <f xml:space="preserve"> 100-71.66</f>
-        <v>28.340000000000003</v>
+        <v>29.3</v>
       </c>
       <c r="M37">
-        <f>100-56.41</f>
-        <v>43.59</v>
+        <v>29.3</v>
       </c>
       <c r="N37">
-        <f>100-56.41</f>
-        <v>43.59</v>
+        <v>29.3</v>
       </c>
       <c r="O37">
         <v>1.7443199999999999E-3</v>
       </c>
       <c r="P37">
-        <v>1</v>
+        <v>6.0059199999999997</v>
       </c>
     </row>
     <row r="38" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
-        <v>45</v>
+        <v>85</v>
       </c>
       <c r="B38">
         <v>0</v>
@@ -2594,16 +2560,16 @@
       <c r="E38">
         <v>0</v>
       </c>
-      <c r="F38" s="10">
+      <c r="F38" s="1">
         <v>50</v>
       </c>
-      <c r="G38" s="10">
+      <c r="G38" s="1">
         <v>95</v>
       </c>
-      <c r="H38" s="10">
-        <v>0</v>
-      </c>
-      <c r="I38" s="10">
+      <c r="H38" s="1">
+        <v>0</v>
+      </c>
+      <c r="I38" s="1">
         <v>0</v>
       </c>
       <c r="J38">
@@ -2633,7 +2599,7 @@
     </row>
     <row r="39" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="B39">
         <v>12.53120360861462</v>
@@ -2647,16 +2613,16 @@
       <c r="E39">
         <v>0</v>
       </c>
-      <c r="F39" s="32">
-        <v>0</v>
-      </c>
-      <c r="G39" s="32">
-        <v>0</v>
-      </c>
-      <c r="H39" s="32">
-        <v>0</v>
-      </c>
-      <c r="I39" s="32">
+      <c r="F39" s="1">
+        <v>0</v>
+      </c>
+      <c r="G39" s="1">
+        <v>0</v>
+      </c>
+      <c r="H39" s="1">
+        <v>0</v>
+      </c>
+      <c r="I39" s="1">
         <v>0</v>
       </c>
       <c r="J39">
@@ -2683,7 +2649,7 @@
     </row>
     <row r="40" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="B40">
         <v>0</v>
@@ -2697,16 +2663,16 @@
       <c r="E40">
         <v>0</v>
       </c>
-      <c r="F40" s="32">
-        <v>0</v>
-      </c>
-      <c r="G40" s="32">
-        <v>0</v>
-      </c>
-      <c r="H40" s="32">
-        <v>0</v>
-      </c>
-      <c r="I40" s="32">
+      <c r="F40" s="1">
+        <v>0</v>
+      </c>
+      <c r="G40" s="1">
+        <v>0</v>
+      </c>
+      <c r="H40" s="1">
+        <v>0</v>
+      </c>
+      <c r="I40" s="1">
         <v>0</v>
       </c>
       <c r="J40">
@@ -2733,7 +2699,7 @@
     </row>
     <row r="41" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="B41">
         <v>0</v>
@@ -2747,16 +2713,16 @@
       <c r="E41">
         <v>0</v>
       </c>
-      <c r="F41" s="32">
-        <v>0</v>
-      </c>
-      <c r="G41" s="32">
-        <v>0</v>
-      </c>
-      <c r="H41" s="32">
-        <v>0</v>
-      </c>
-      <c r="I41" s="32">
+      <c r="F41" s="1">
+        <v>0</v>
+      </c>
+      <c r="G41" s="1">
+        <v>0</v>
+      </c>
+      <c r="H41" s="1">
+        <v>0</v>
+      </c>
+      <c r="I41" s="1">
         <v>0</v>
       </c>
       <c r="J41">
@@ -2783,61 +2749,57 @@
     </row>
     <row r="42" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
-        <v>49</v>
+        <v>82</v>
       </c>
       <c r="B42">
-        <v>10</v>
+        <v>4.5</v>
       </c>
       <c r="C42">
-        <v>0</v>
+        <v>1.4</v>
       </c>
       <c r="D42">
         <v>0</v>
       </c>
       <c r="E42">
-        <v>0</v>
-      </c>
-      <c r="F42" s="32">
-        <v>58.62</v>
-      </c>
-      <c r="G42" s="32">
-        <v>92.13</v>
-      </c>
-      <c r="H42" s="32">
+        <v>0.5</v>
+      </c>
+      <c r="F42" s="1">
         <v>50</v>
       </c>
-      <c r="I42" s="32">
-        <v>52.88</v>
+      <c r="G42" s="1">
+        <v>95</v>
+      </c>
+      <c r="H42" s="1">
+        <v>0</v>
+      </c>
+      <c r="I42" s="1">
+        <v>0</v>
       </c>
       <c r="J42">
         <v>0</v>
       </c>
       <c r="K42">
-        <f>100-100*0.855117</f>
-        <v>14.488299999999995</v>
+        <v>16</v>
       </c>
       <c r="L42">
-        <f>100-100*0.836</f>
-        <v>16.400000000000006</v>
+        <v>24</v>
       </c>
       <c r="M42">
-        <f>100-100*0.46</f>
-        <v>54</v>
+        <v>45.5</v>
       </c>
       <c r="N42">
-        <f>100-100*0.46</f>
-        <v>54</v>
+        <v>45.5</v>
       </c>
       <c r="O42">
-        <v>1.08877E-2</v>
+        <v>8.3131800000000006E-2</v>
       </c>
       <c r="P42">
-        <v>3.07</v>
+        <v>14.065899999999999</v>
       </c>
     </row>
     <row r="43" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="B43">
         <v>0</v>
@@ -2851,16 +2813,16 @@
       <c r="E43" s="1">
         <v>10</v>
       </c>
-      <c r="F43" s="11">
+      <c r="F43" s="1">
         <v>70</v>
       </c>
-      <c r="G43" s="11">
+      <c r="G43" s="1">
         <v>95</v>
       </c>
-      <c r="H43" s="11">
+      <c r="H43" s="1">
         <v>90</v>
       </c>
-      <c r="I43" s="11">
+      <c r="I43" s="1">
         <v>90</v>
       </c>
       <c r="J43">
@@ -2887,7 +2849,7 @@
     </row>
     <row r="44" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="B44">
         <v>0</v>
@@ -2901,16 +2863,16 @@
       <c r="E44">
         <v>0</v>
       </c>
-      <c r="F44" s="12">
+      <c r="F44" s="1">
         <v>70</v>
       </c>
-      <c r="G44" s="12">
+      <c r="G44" s="1">
         <v>95</v>
       </c>
-      <c r="H44" s="12">
+      <c r="H44" s="1">
         <v>90</v>
       </c>
-      <c r="I44" s="12">
+      <c r="I44" s="1">
         <v>90</v>
       </c>
       <c r="J44">
@@ -2937,7 +2899,7 @@
     </row>
     <row r="45" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="B45">
         <v>0</v>
@@ -2951,16 +2913,16 @@
       <c r="E45">
         <v>0</v>
       </c>
-      <c r="F45" s="32">
-        <v>0</v>
-      </c>
-      <c r="G45" s="32">
-        <v>0</v>
-      </c>
-      <c r="H45" s="32">
-        <v>0</v>
-      </c>
-      <c r="I45" s="32">
+      <c r="F45" s="1">
+        <v>0</v>
+      </c>
+      <c r="G45" s="1">
+        <v>0</v>
+      </c>
+      <c r="H45" s="1">
+        <v>0</v>
+      </c>
+      <c r="I45" s="1">
         <v>0</v>
       </c>
       <c r="J45">
@@ -2987,7 +2949,7 @@
     </row>
     <row r="46" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="B46" s="1">
         <v>10</v>
@@ -3001,16 +2963,16 @@
       <c r="E46">
         <v>0</v>
       </c>
-      <c r="F46" s="32">
-        <v>0</v>
-      </c>
-      <c r="G46" s="32">
-        <v>0</v>
-      </c>
-      <c r="H46" s="32">
-        <v>0</v>
-      </c>
-      <c r="I46" s="32">
+      <c r="F46" s="1">
+        <v>0</v>
+      </c>
+      <c r="G46" s="1">
+        <v>0</v>
+      </c>
+      <c r="H46" s="1">
+        <v>0</v>
+      </c>
+      <c r="I46" s="1">
         <v>0</v>
       </c>
       <c r="J46">
@@ -3037,7 +2999,7 @@
     </row>
     <row r="47" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="B47">
         <v>0</v>
@@ -3051,16 +3013,16 @@
       <c r="E47">
         <v>0</v>
       </c>
-      <c r="F47" s="32">
-        <v>0</v>
-      </c>
-      <c r="G47" s="32">
-        <v>0</v>
-      </c>
-      <c r="H47" s="32">
-        <v>0</v>
-      </c>
-      <c r="I47" s="32">
+      <c r="F47" s="1">
+        <v>0</v>
+      </c>
+      <c r="G47" s="1">
+        <v>0</v>
+      </c>
+      <c r="H47" s="1">
+        <v>0</v>
+      </c>
+      <c r="I47" s="1">
         <v>0</v>
       </c>
       <c r="J47">
@@ -3087,7 +3049,7 @@
     </row>
     <row r="48" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="B48">
         <v>0</v>
@@ -3101,16 +3063,16 @@
       <c r="E48">
         <v>0</v>
       </c>
-      <c r="F48" s="32">
-        <v>0</v>
-      </c>
-      <c r="G48" s="32">
-        <v>0</v>
-      </c>
-      <c r="H48" s="32">
-        <v>0</v>
-      </c>
-      <c r="I48" s="32">
+      <c r="F48" s="1">
+        <v>0</v>
+      </c>
+      <c r="G48" s="1">
+        <v>0</v>
+      </c>
+      <c r="H48" s="1">
+        <v>0</v>
+      </c>
+      <c r="I48" s="1">
         <v>0</v>
       </c>
       <c r="J48">
@@ -3137,7 +3099,7 @@
     </row>
     <row r="49" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="B49">
         <v>13.439860216496591</v>
@@ -3151,16 +3113,16 @@
       <c r="E49" s="1">
         <v>10</v>
       </c>
-      <c r="F49" s="32">
-        <v>0</v>
-      </c>
-      <c r="G49" s="32">
-        <v>0</v>
-      </c>
-      <c r="H49" s="32">
-        <v>0</v>
-      </c>
-      <c r="I49" s="32">
+      <c r="F49" s="1">
+        <v>0</v>
+      </c>
+      <c r="G49" s="1">
+        <v>0</v>
+      </c>
+      <c r="H49" s="1">
+        <v>0</v>
+      </c>
+      <c r="I49" s="1">
         <v>0</v>
       </c>
       <c r="J49">
@@ -3187,7 +3149,7 @@
     </row>
     <row r="50" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="B50">
         <v>40.296471341616311</v>
@@ -3201,16 +3163,16 @@
       <c r="E50" s="1">
         <v>10</v>
       </c>
-      <c r="F50" s="14">
+      <c r="F50">
         <v>90</v>
       </c>
-      <c r="G50" s="13">
+      <c r="G50" s="1">
         <v>98</v>
       </c>
-      <c r="H50" s="13">
+      <c r="H50" s="1">
         <v>90</v>
       </c>
-      <c r="I50" s="14">
+      <c r="I50">
         <v>91</v>
       </c>
       <c r="J50">
@@ -3237,7 +3199,7 @@
     </row>
     <row r="51" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="B51">
         <v>17.138720782557488</v>
@@ -3251,16 +3213,16 @@
       <c r="E51">
         <v>0</v>
       </c>
-      <c r="F51" s="32">
-        <v>0</v>
-      </c>
-      <c r="G51" s="32">
-        <v>0</v>
-      </c>
-      <c r="H51" s="32">
-        <v>0</v>
-      </c>
-      <c r="I51" s="32">
+      <c r="F51" s="1">
+        <v>0</v>
+      </c>
+      <c r="G51" s="1">
+        <v>0</v>
+      </c>
+      <c r="H51" s="1">
+        <v>0</v>
+      </c>
+      <c r="I51" s="1">
         <v>0</v>
       </c>
       <c r="J51">
@@ -3287,7 +3249,7 @@
     </row>
     <row r="52" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="B52">
         <v>0</v>
@@ -3301,16 +3263,16 @@
       <c r="E52">
         <v>0</v>
       </c>
-      <c r="F52" s="32">
-        <v>0</v>
-      </c>
-      <c r="G52" s="32">
-        <v>0</v>
-      </c>
-      <c r="H52" s="32">
-        <v>0</v>
-      </c>
-      <c r="I52" s="32">
+      <c r="F52" s="1">
+        <v>0</v>
+      </c>
+      <c r="G52" s="1">
+        <v>0</v>
+      </c>
+      <c r="H52" s="1">
+        <v>0</v>
+      </c>
+      <c r="I52" s="1">
         <v>0</v>
       </c>
       <c r="J52">
@@ -3337,30 +3299,30 @@
     </row>
     <row r="53" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
+        <v>53</v>
+      </c>
+      <c r="B53">
+        <v>0</v>
+      </c>
+      <c r="C53">
+        <v>0</v>
+      </c>
+      <c r="D53">
+        <v>0</v>
+      </c>
+      <c r="E53">
+        <v>0</v>
+      </c>
+      <c r="F53" s="1">
+        <v>30</v>
+      </c>
+      <c r="G53" s="1">
+        <v>70</v>
+      </c>
+      <c r="H53" s="1">
         <v>60</v>
       </c>
-      <c r="B53">
-        <v>0</v>
-      </c>
-      <c r="C53">
-        <v>0</v>
-      </c>
-      <c r="D53">
-        <v>0</v>
-      </c>
-      <c r="E53">
-        <v>0</v>
-      </c>
-      <c r="F53" s="15">
-        <v>30</v>
-      </c>
-      <c r="G53" s="15">
-        <v>70</v>
-      </c>
-      <c r="H53" s="15">
-        <v>60</v>
-      </c>
-      <c r="I53" s="16">
+      <c r="I53">
         <v>94</v>
       </c>
       <c r="J53">
@@ -3387,7 +3349,7 @@
     </row>
     <row r="54" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="B54">
         <v>0</v>
@@ -3401,16 +3363,16 @@
       <c r="E54">
         <v>0</v>
       </c>
-      <c r="F54" s="32">
-        <v>0</v>
-      </c>
-      <c r="G54" s="32">
-        <v>0</v>
-      </c>
-      <c r="H54" s="32">
-        <v>0</v>
-      </c>
-      <c r="I54" s="32">
+      <c r="F54" s="1">
+        <v>0</v>
+      </c>
+      <c r="G54" s="1">
+        <v>0</v>
+      </c>
+      <c r="H54" s="1">
+        <v>0</v>
+      </c>
+      <c r="I54" s="1">
         <v>0</v>
       </c>
       <c r="J54">
@@ -3437,7 +3399,7 @@
     </row>
     <row r="55" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="B55">
         <v>0</v>
@@ -3451,16 +3413,16 @@
       <c r="E55">
         <v>0</v>
       </c>
-      <c r="F55" s="32">
-        <v>0</v>
-      </c>
-      <c r="G55" s="32">
-        <v>0</v>
-      </c>
-      <c r="H55" s="32">
-        <v>0</v>
-      </c>
-      <c r="I55" s="32">
+      <c r="F55" s="1">
+        <v>0</v>
+      </c>
+      <c r="G55" s="1">
+        <v>0</v>
+      </c>
+      <c r="H55" s="1">
+        <v>0</v>
+      </c>
+      <c r="I55" s="1">
         <v>0</v>
       </c>
       <c r="J55">
@@ -3487,13 +3449,13 @@
     </row>
     <row r="56" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="B56">
         <v>0</v>
       </c>
       <c r="C56">
-        <v>0</v>
+        <v>1.5</v>
       </c>
       <c r="D56">
         <v>0</v>
@@ -3501,47 +3463,43 @@
       <c r="E56">
         <v>0</v>
       </c>
-      <c r="F56" s="17">
+      <c r="F56" s="1">
         <v>30</v>
       </c>
-      <c r="G56" s="17">
+      <c r="G56" s="1">
         <v>50</v>
       </c>
-      <c r="H56" s="17">
+      <c r="H56" s="1">
         <v>30</v>
       </c>
-      <c r="I56" s="18">
+      <c r="I56">
         <v>25</v>
       </c>
       <c r="J56">
         <v>0</v>
       </c>
       <c r="K56">
-        <f>100-100*0.978</f>
-        <v>2.2000000000000028</v>
+        <v>1.96</v>
       </c>
       <c r="L56">
-        <f>100-100*0.405655</f>
-        <v>59.4345</v>
+        <v>69.63</v>
       </c>
       <c r="M56">
-        <f>100-100*0.405655</f>
-        <v>59.4345</v>
+        <v>69.63</v>
       </c>
       <c r="N56">
-        <f>100-100*0.405655</f>
-        <v>59.4345</v>
+        <v>69.930000000000007</v>
       </c>
       <c r="O56">
-        <v>8.5849400000000001E-4</v>
+        <v>9.25872E-4</v>
       </c>
       <c r="P56">
-        <v>1</v>
+        <v>1.0776399999999999</v>
       </c>
     </row>
     <row r="57" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="B57">
         <v>78.927457572534323</v>
@@ -3555,16 +3513,16 @@
       <c r="E57">
         <v>0</v>
       </c>
-      <c r="F57" s="32">
-        <v>0</v>
-      </c>
-      <c r="G57" s="32">
-        <v>0</v>
-      </c>
-      <c r="H57" s="32">
-        <v>0</v>
-      </c>
-      <c r="I57" s="32">
+      <c r="F57" s="1">
+        <v>0</v>
+      </c>
+      <c r="G57" s="1">
+        <v>0</v>
+      </c>
+      <c r="H57" s="1">
+        <v>0</v>
+      </c>
+      <c r="I57" s="1">
         <v>0</v>
       </c>
       <c r="J57">
@@ -3591,7 +3549,7 @@
     </row>
     <row r="58" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="B58">
         <v>0.39067434019214309</v>
@@ -3605,16 +3563,16 @@
       <c r="E58" s="1">
         <v>10</v>
       </c>
-      <c r="F58" s="19">
+      <c r="F58" s="1">
         <v>90</v>
       </c>
-      <c r="G58" s="19">
+      <c r="G58" s="1">
         <v>98</v>
       </c>
-      <c r="H58" s="19">
+      <c r="H58" s="1">
         <v>80</v>
       </c>
-      <c r="I58" s="20">
+      <c r="I58">
         <v>67</v>
       </c>
       <c r="J58">
@@ -3641,7 +3599,7 @@
     </row>
     <row r="59" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="B59">
         <v>1.906421316019979</v>
@@ -3655,16 +3613,16 @@
       <c r="E59">
         <v>0</v>
       </c>
-      <c r="F59" s="22">
+      <c r="F59">
         <v>85</v>
       </c>
-      <c r="G59" s="21">
+      <c r="G59" s="1">
         <v>98</v>
       </c>
-      <c r="H59" s="21">
+      <c r="H59" s="1">
         <v>80</v>
       </c>
-      <c r="I59" s="22">
+      <c r="I59">
         <v>89</v>
       </c>
       <c r="J59" s="1">
@@ -3691,7 +3649,7 @@
     </row>
     <row r="60" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="B60">
         <v>0</v>
@@ -3705,16 +3663,16 @@
       <c r="E60">
         <v>0</v>
       </c>
-      <c r="F60" s="32">
-        <v>0</v>
-      </c>
-      <c r="G60" s="32">
-        <v>0</v>
-      </c>
-      <c r="H60" s="32">
-        <v>0</v>
-      </c>
-      <c r="I60" s="32">
+      <c r="F60" s="1">
+        <v>0</v>
+      </c>
+      <c r="G60" s="1">
+        <v>0</v>
+      </c>
+      <c r="H60" s="1">
+        <v>0</v>
+      </c>
+      <c r="I60" s="1">
         <v>0</v>
       </c>
       <c r="J60">
@@ -3741,7 +3699,7 @@
     </row>
     <row r="61" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
-        <v>68</v>
+        <v>83</v>
       </c>
       <c r="B61">
         <v>0</v>
@@ -3755,16 +3713,16 @@
       <c r="E61">
         <v>0</v>
       </c>
-      <c r="F61" s="24">
+      <c r="F61">
         <v>55</v>
       </c>
-      <c r="G61" s="23">
+      <c r="G61" s="1">
         <v>98</v>
       </c>
-      <c r="H61" s="23">
-        <v>0</v>
-      </c>
-      <c r="I61" s="23">
+      <c r="H61" s="1">
+        <v>0</v>
+      </c>
+      <c r="I61" s="1">
         <v>0</v>
       </c>
       <c r="J61">
@@ -3795,7 +3753,7 @@
     </row>
     <row r="62" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="B62">
         <v>0</v>
@@ -3809,16 +3767,16 @@
       <c r="E62" s="1">
         <v>0</v>
       </c>
-      <c r="F62" s="25">
+      <c r="F62" s="1">
         <v>40</v>
       </c>
-      <c r="G62" s="25">
+      <c r="G62" s="1">
         <v>99</v>
       </c>
-      <c r="H62" s="25">
+      <c r="H62" s="1">
         <v>40</v>
       </c>
-      <c r="I62" s="25">
+      <c r="I62" s="1">
         <v>20</v>
       </c>
       <c r="J62">
@@ -3845,7 +3803,7 @@
     </row>
     <row r="63" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
       <c r="B63">
         <v>0</v>
@@ -3859,16 +3817,16 @@
       <c r="E63" s="1">
         <v>0</v>
       </c>
-      <c r="F63" s="27">
+      <c r="F63" s="1">
         <v>30</v>
       </c>
-      <c r="G63" s="27">
+      <c r="G63" s="1">
         <v>95</v>
       </c>
-      <c r="H63" s="27">
+      <c r="H63" s="1">
         <v>20</v>
       </c>
-      <c r="I63" s="27">
+      <c r="I63" s="1">
         <v>10</v>
       </c>
       <c r="J63">
@@ -3895,7 +3853,7 @@
     </row>
     <row r="64" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
       <c r="B64">
         <v>0</v>
@@ -3909,16 +3867,16 @@
       <c r="E64" s="1">
         <v>0</v>
       </c>
-      <c r="F64" s="26">
+      <c r="F64" s="1">
         <v>30</v>
       </c>
-      <c r="G64" s="26">
+      <c r="G64" s="1">
         <v>95</v>
       </c>
-      <c r="H64" s="26">
+      <c r="H64" s="1">
         <v>20</v>
       </c>
-      <c r="I64" s="26">
+      <c r="I64" s="1">
         <v>10</v>
       </c>
       <c r="J64">
@@ -3945,7 +3903,7 @@
     </row>
     <row r="65" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
       <c r="B65">
         <v>0</v>
@@ -3959,16 +3917,16 @@
       <c r="E65">
         <v>0</v>
       </c>
-      <c r="F65" s="31">
+      <c r="F65" s="1">
         <v>10</v>
       </c>
-      <c r="G65" s="31">
+      <c r="G65" s="1">
         <v>99</v>
       </c>
-      <c r="H65" s="31">
-        <v>0</v>
-      </c>
-      <c r="I65" s="31">
+      <c r="H65" s="1">
+        <v>0</v>
+      </c>
+      <c r="I65" s="1">
         <v>0</v>
       </c>
       <c r="J65">
@@ -3995,7 +3953,7 @@
     </row>
     <row r="66" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
       <c r="B66">
         <v>0</v>
@@ -4009,16 +3967,16 @@
       <c r="E66">
         <v>0</v>
       </c>
-      <c r="F66" s="32">
+      <c r="F66" s="1">
         <v>10</v>
       </c>
-      <c r="G66" s="32">
+      <c r="G66" s="1">
         <v>99</v>
       </c>
-      <c r="H66" s="32">
-        <v>0</v>
-      </c>
-      <c r="I66" s="32">
+      <c r="H66" s="1">
+        <v>0</v>
+      </c>
+      <c r="I66" s="1">
         <v>0</v>
       </c>
       <c r="J66">
@@ -4045,7 +4003,7 @@
     </row>
     <row r="67" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="B67">
         <v>0</v>
@@ -4059,16 +4017,16 @@
       <c r="E67" s="1">
         <v>0</v>
       </c>
-      <c r="F67" s="28">
+      <c r="F67" s="1">
         <v>30</v>
       </c>
-      <c r="G67" s="28">
+      <c r="G67" s="1">
         <v>95</v>
       </c>
-      <c r="H67" s="28">
+      <c r="H67" s="1">
         <v>20</v>
       </c>
-      <c r="I67" s="28">
+      <c r="I67" s="1">
         <v>10</v>
       </c>
       <c r="J67">
@@ -4095,7 +4053,7 @@
     </row>
     <row r="68" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="B68">
         <v>0</v>
@@ -4109,16 +4067,16 @@
       <c r="E68">
         <v>0</v>
       </c>
-      <c r="F68" s="30">
+      <c r="F68" s="1">
         <v>10</v>
       </c>
-      <c r="G68" s="30">
+      <c r="G68" s="1">
         <v>99</v>
       </c>
-      <c r="H68" s="30">
-        <v>0</v>
-      </c>
-      <c r="I68" s="30">
+      <c r="H68" s="1">
+        <v>0</v>
+      </c>
+      <c r="I68" s="1">
         <v>0</v>
       </c>
       <c r="J68">
@@ -4145,7 +4103,7 @@
     </row>
     <row r="69" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
       <c r="B69">
         <v>0</v>
@@ -4159,16 +4117,16 @@
       <c r="E69" s="1">
         <v>0</v>
       </c>
-      <c r="F69" s="32">
+      <c r="F69" s="1">
         <v>30</v>
       </c>
-      <c r="G69" s="32">
+      <c r="G69" s="1">
         <v>95</v>
       </c>
-      <c r="H69" s="32">
+      <c r="H69" s="1">
         <v>20</v>
       </c>
-      <c r="I69" s="32">
+      <c r="I69" s="1">
         <v>10</v>
       </c>
       <c r="J69">
@@ -4195,7 +4153,7 @@
     </row>
     <row r="70" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="B70">
         <v>0</v>
@@ -4209,16 +4167,16 @@
       <c r="E70">
         <v>0</v>
       </c>
-      <c r="F70" s="32">
-        <v>0</v>
-      </c>
-      <c r="G70" s="32">
-        <v>0</v>
-      </c>
-      <c r="H70" s="32">
-        <v>0</v>
-      </c>
-      <c r="I70" s="32">
+      <c r="F70" s="1">
+        <v>0</v>
+      </c>
+      <c r="G70" s="1">
+        <v>0</v>
+      </c>
+      <c r="H70" s="1">
+        <v>0</v>
+      </c>
+      <c r="I70" s="1">
         <v>0</v>
       </c>
       <c r="J70">
@@ -4245,7 +4203,7 @@
     </row>
     <row r="71" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="B71">
         <v>0</v>
@@ -4259,16 +4217,16 @@
       <c r="E71" s="1">
         <v>0</v>
       </c>
-      <c r="F71" s="29">
+      <c r="F71" s="1">
         <v>30</v>
       </c>
-      <c r="G71" s="29">
+      <c r="G71" s="1">
         <v>95</v>
       </c>
-      <c r="H71" s="29">
+      <c r="H71" s="1">
         <v>20</v>
       </c>
-      <c r="I71" s="29">
+      <c r="I71" s="1">
         <v>10</v>
       </c>
       <c r="J71">

</xml_diff>